<commit_message>
Initial commit: Lab automation framework with enhanced bridge domain discovery and P2MP capabilities
</commit_message>
<xml_diff>
--- a/inventory/DNAAS Inventory.xlsx
+++ b/inventory/DNAAS Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slavaisaev/Cursor_scripts /lab_automation/inventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://drivenets-my.sharepoint.com/personal/nchuosho_drivenets_com/Documents/shared/IL LAB/ICT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A00975F-98CD-F947-8035-2476CD78F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B1CB85D-4447-471A-8491-42127B603083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34160" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19200" yWindow="0" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="255">
   <si>
     <t>Index</t>
   </si>
@@ -168,6 +168,642 @@
   </si>
   <si>
     <t>100.64.101.21</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A10</t>
+  </si>
+  <si>
+    <t>wdy1c8v30007b</t>
+  </si>
+  <si>
+    <t>100.64.101.22</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A11-1</t>
+  </si>
+  <si>
+    <t>wdy1c8v300097</t>
+  </si>
+  <si>
+    <t>100.64.101.14</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A11-2</t>
+  </si>
+  <si>
+    <t>wdy1c8vh00015</t>
+  </si>
+  <si>
+    <t>100.64.101.15</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A12</t>
+  </si>
+  <si>
+    <t>wdy1c8vy00093</t>
+  </si>
+  <si>
+    <t>100.64.101.17</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A13</t>
+  </si>
+  <si>
+    <t>wdy1c8v000094</t>
+  </si>
+  <si>
+    <t>100.64.101.31</t>
+  </si>
+  <si>
+    <t>7 (2nd E2E)</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A14</t>
+  </si>
+  <si>
+    <t>wdy1c8v0000b0</t>
+  </si>
+  <si>
+    <t>100.64.101.32</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A15</t>
+  </si>
+  <si>
+    <t>wdy1c3v00006d</t>
+  </si>
+  <si>
+    <t>100.64.101.16</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-A16</t>
+  </si>
+  <si>
+    <t>wdy1c3v10006e</t>
+  </si>
+  <si>
+    <t>100.64.101.33</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B01</t>
+  </si>
+  <si>
+    <t>wdy1d2vg00016</t>
+  </si>
+  <si>
+    <t>100.64.101.34</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B02</t>
+  </si>
+  <si>
+    <t>wdy1d2vd00005</t>
+  </si>
+  <si>
+    <t>100.64.101.35</t>
+  </si>
+  <si>
+    <t>B03</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B03</t>
+  </si>
+  <si>
+    <t>wdy1d2vf00007</t>
+  </si>
+  <si>
+    <t>100.64.101.36</t>
+  </si>
+  <si>
+    <t>B04</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B04</t>
+  </si>
+  <si>
+    <t>wdy1cav000024</t>
+  </si>
+  <si>
+    <t>100.64.101.37</t>
+  </si>
+  <si>
+    <t>B05</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B05</t>
+  </si>
+  <si>
+    <t>wdy1c8v3000b3</t>
+  </si>
+  <si>
+    <t>100.64.101.38</t>
+  </si>
+  <si>
+    <t>B06</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B06-1</t>
+  </si>
+  <si>
+    <t>wdy1d2vj0000a</t>
+  </si>
+  <si>
+    <t>100.64.101.39</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B06-2 (NCPL)</t>
+  </si>
+  <si>
+    <t>wng1c7vl00012p2</t>
+  </si>
+  <si>
+    <t>100.64.101.40</t>
+  </si>
+  <si>
+    <t>B07</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B07</t>
+  </si>
+  <si>
+    <t>wdy1d2vh00009</t>
+  </si>
+  <si>
+    <t>100.64.101.2</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B10</t>
+  </si>
+  <si>
+    <t>wdy1c8vv00082</t>
+  </si>
+  <si>
+    <t>100.64.101.3</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B13</t>
+  </si>
+  <si>
+    <t>wdy1c8vn00036</t>
+  </si>
+  <si>
+    <t>100.64.101.4</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B14</t>
+  </si>
+  <si>
+    <t>wdy1cav400052</t>
+  </si>
+  <si>
+    <t>100.64.101.5</t>
+  </si>
+  <si>
+    <t>B15</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B15</t>
+  </si>
+  <si>
+    <t>wdy1c8vv00090</t>
+  </si>
+  <si>
+    <t>100.64.101.6</t>
+  </si>
+  <si>
+    <t>B16</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-B16</t>
+  </si>
+  <si>
+    <t>wdy1c8v60007e</t>
+  </si>
+  <si>
+    <t>100.64.101.7</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C01</t>
+  </si>
+  <si>
+    <t>wdy1a77w00040</t>
+  </si>
+  <si>
+    <t>100.64.101.41</t>
+  </si>
+  <si>
+    <t>not deployed yet</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C02</t>
+  </si>
+  <si>
+    <t>wdw1b87j00002</t>
+  </si>
+  <si>
+    <t>100.64.101.42</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C03</t>
+  </si>
+  <si>
+    <t>wdy1c8v20006c</t>
+  </si>
+  <si>
+    <t>100.64.101.43</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C04</t>
+  </si>
+  <si>
+    <t>wdy1c9vd000c4</t>
+  </si>
+  <si>
+    <t>100.64.101.44</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C05</t>
+  </si>
+  <si>
+    <t>wdy1a77x00033</t>
+  </si>
+  <si>
+    <t>100.64.101.45</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C06</t>
+  </si>
+  <si>
+    <t>wdy1b47d00013</t>
+  </si>
+  <si>
+    <t>100.64.101.46</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C07</t>
+  </si>
+  <si>
+    <t>wdy1c8vp00037</t>
+  </si>
+  <si>
+    <t>100.64.101.47</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C10</t>
+  </si>
+  <si>
+    <t>wdy1a77v00031</t>
+  </si>
+  <si>
+    <t>100.64.101.8</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C11</t>
+  </si>
+  <si>
+    <t>wdy1c8v40006e</t>
+  </si>
+  <si>
+    <t>100.64.101.9</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C12-A</t>
+  </si>
+  <si>
+    <t>wdy1d2vh00017</t>
+  </si>
+  <si>
+    <t>100.64.101.10</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C12-B</t>
+  </si>
+  <si>
+    <t>WDY1CAVW00021</t>
+  </si>
+  <si>
+    <t>100.64.101.11</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C13</t>
+  </si>
+  <si>
+    <t>wdy1d2vf00015</t>
+  </si>
+  <si>
+    <t>100.64.101.53</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C14</t>
+  </si>
+  <si>
+    <t>wdy1d2vc00012</t>
+  </si>
+  <si>
+    <t>100.64.101.54</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C15</t>
+  </si>
+  <si>
+    <t>wdy1c3vv00069</t>
+  </si>
+  <si>
+    <t>100.64.101.55</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-C16</t>
+  </si>
+  <si>
+    <t>wdy1d2ve00014</t>
+  </si>
+  <si>
+    <t>100.64.101.56</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-D12</t>
+  </si>
+  <si>
+    <t>WK31D8V700019</t>
+  </si>
+  <si>
+    <t>100.64.101.51</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>DNAAS_LEAF_D13</t>
+  </si>
+  <si>
+    <t>wdy1cavb00059</t>
+  </si>
+  <si>
+    <t>100.64.101.52</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>DNAAS_LEAF_D15</t>
+  </si>
+  <si>
+    <t>WK31D8V500017</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>DNAAS_LEAF_D16</t>
+  </si>
+  <si>
+    <t>wdy1c8vt00072</t>
+  </si>
+  <si>
+    <t>100.64.101.123</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-F14</t>
+  </si>
+  <si>
+    <t>wdy1d1vf0002a</t>
+  </si>
+  <si>
+    <t>100.64.101.57</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-F15</t>
+  </si>
+  <si>
+    <t>wdy1cav80002c</t>
+  </si>
+  <si>
+    <t>100.64.101.58</t>
+  </si>
+  <si>
+    <t>F16</t>
+  </si>
+  <si>
+    <t>DNAAS-LEAF-F16</t>
+  </si>
+  <si>
+    <t>wdy1cave0005c</t>
+  </si>
+  <si>
+    <t>100.64.101.59</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-A08</t>
+  </si>
+  <si>
+    <t>wdy1c8v000078</t>
+  </si>
+  <si>
+    <t>100.64.100.134</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-A09</t>
+  </si>
+  <si>
+    <t>wdy1c8vx00076</t>
+  </si>
+  <si>
+    <t>100.64.100.128</t>
+  </si>
+  <si>
+    <t>B08</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-B08</t>
+  </si>
+  <si>
+    <t>wdy1c8v70007f</t>
+  </si>
+  <si>
+    <t>100.64.100.130</t>
+  </si>
+  <si>
+    <t>B09</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-B09</t>
+  </si>
+  <si>
+    <t>wdy1cavx00022</t>
+  </si>
+  <si>
+    <t>100.64.100.12</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-C08</t>
+  </si>
+  <si>
+    <t>wdw1bbvf0000c</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-C09</t>
+  </si>
+  <si>
+    <t>wdy1b77e0001f</t>
+  </si>
+  <si>
+    <t>100.64.100.251</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>DNAAS_SPINE_D14</t>
+  </si>
+  <si>
+    <t>wdy1c8v2000b2</t>
+  </si>
+  <si>
+    <t>100.64.100.129</t>
+  </si>
+  <si>
+    <t>F09</t>
+  </si>
+  <si>
+    <t>DNAAS-SPINE-F09</t>
+  </si>
+  <si>
+    <t>wdy1cavh0005f</t>
+  </si>
+  <si>
+    <t>100.64.100.131</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>DNAAS-SuperSpine-D04-NCC0</t>
+  </si>
+  <si>
+    <t>CZJ2130SW0</t>
+  </si>
+  <si>
+    <t>100.64.100.1</t>
+  </si>
+  <si>
+    <t>DNAAS-SuperSpine-D04-NCC1</t>
+  </si>
+  <si>
+    <t>CZJ2130SVL</t>
+  </si>
+  <si>
+    <t>נאור תעשה לי זיקוקים בחודידה</t>
+  </si>
+  <si>
+    <t>נאור יא גברררר</t>
+  </si>
+  <si>
+    <t>נאור תעשה לי ילדים</t>
+  </si>
+  <si>
+    <t>נאור המלך!!!!!</t>
   </si>
 </sst>
 </file>
@@ -204,7 +840,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -602,6 +1237,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -618,13 +1260,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -669,7 +1304,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE3C091D-A8BE-3740-98C7-457ECDE2706E}" name="Table2" displayName="Table2" ref="A1:I62" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE3C091D-A8BE-3740-98C7-457ECDE2706E}" name="Table2" displayName="Table2" ref="A1:I62" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
   <autoFilter ref="A1:I62" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6978355D-C430-8D45-8E10-2AF44A4782D0}" name="Index" dataDxfId="8"/>
@@ -973,22 +1608,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="2"/>
-    <col min="3" max="3" width="29.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="26.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1253,591 +1888,1468 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G25" s="5"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G26" s="5"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
+      <c r="H27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G28" s="5"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="H28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="16"/>
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="16"/>
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="16"/>
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="16"/>
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="16"/>
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="16"/>
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="16"/>
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G38" s="5"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G39" s="5"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G40" s="5"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G41" s="5"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="H41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="5">
+        <v>70</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="5">
+        <v>70</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="5">
+        <v>70</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="5">
+        <v>70</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="8"/>
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G46" s="5"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="8"/>
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G47" s="5"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="16"/>
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G49" s="5"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="5">
+        <v>70</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="5">
+        <v>70</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="5">
+        <v>70</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="8"/>
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G55" s="5"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
+      <c r="H55" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="8"/>
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G56" s="5"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
+      <c r="H56" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="16"/>
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="8"/>
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G58" s="5"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
+      <c r="H58" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="8"/>
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G59" s="5"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
+      <c r="H59" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="5">
+        <v>70</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="65" spans="3:16">
-      <c r="C65" s="4"/>
+      <c r="C65" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>

</xml_diff>